<commit_message>
fix add option func,more convenient
</commit_message>
<xml_diff>
--- a/test_file/pull_down.xlsx
+++ b/test_file/pull_down.xlsx
@@ -15,14 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>填表说明：
-1. 请严格按照本模板填写导入用户信息，不要修改表头信息（本表1、2行）
-2. 用户姓名、手机号是必填项。用户姓名需在2 - 30个字符之间，头尾不允许空格；手机号按照11位手机号填写，头尾不允许空格，不需加国家码前缀。
-3. 身份证为非必填项。若需填写请严格按照国家有效身份证填写，头尾不允许空格。
-4. 用户组为非必填项。用户组名称需在2 - 30个字符之间，头尾不允许空格。若填写此项，则代表该用户加入指定用户组。若该用户组已经在本机构存在，则意为加入该用户组（不影响现有用户组成员）</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>名称</t>
   </si>
@@ -40,24 +33,23 @@
   </si>
   <si>
     <t>坤</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>world</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="微软雅黑"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -81,14 +73,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="false">
       <alignment/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true" applyProtection="true">
-      <alignment wrapText="true"/>
-      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="false" applyProtection="true">
       <alignment/>
@@ -369,29 +357,24 @@
     <col max="3" min="1" style="1" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" ht="80" customHeight="true">
+    <row r="1" s="2" customFormat="true">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" s="3" customFormat="true">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:X1"/>
-  </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation allowBlank="true" sqref="B2:B3000" type="list">
       <formula1>下拉菜单测试选项数据表!$A$1:$C$1</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="true" sqref="C2:C3000" type="list">
+      <formula1>下拉菜单测试选项数据表!$A$2:$B$2</formula1>
     </dataValidation>
   </dataValidations>
 </worksheet>
@@ -406,13 +389,21 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
         <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>